<commit_message>
second commit: fixed dataset overview and adding readme
</commit_message>
<xml_diff>
--- a/Overview/Overview.xlsx
+++ b/Overview/Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester 7\Temu Kembali Informasi\UTS\Overview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01061D09-E5B2-4281-9DB1-CBD36050EB6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B743BA44-AAF1-4E5D-A405-5DC843F43B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{955E0029-018D-438D-87B5-B0B2BDDFB98F}"/>
   </bookViews>
@@ -135,9 +135,6 @@
     <t>142/Pid.Sus/2024/PN Bjb</t>
   </si>
   <si>
-    <t>1 (satu) Embar plastik klip yang di dalamnya terdapat narkotika jenis sabu-sabu dengan berat kotor seberat 0,17 gram dan berat bersih seberat 0.04 gram; 10 (sepuluh) lembar plastik Kip; 1 (Satu) buah sendok terbuat dari sedotan plastik warna hitam; dan I (satu) lembar plastik warna hitam; Dimusnahkan</t>
-  </si>
-  <si>
     <t>Menyatakan Terdakwa Supiani Alias Amang Bin Ramli, telah terbukti secara sah dan meyakinkan bersalah melakukan tindak pidana “tanpa hak atau melawan hukum menjual Narkotika Golongan I” sebagaimana dalam dakwaan alternatif kesatu; 
 Mahkamah Agung Republik Indonesia Menjatuhkan pidana kepada Terdakwa oleh karena itu dengan pidana penjara selama 6 (enam) tahun 10 (sepuluh) bulan dan pidana denda sejumlah Rp1.000.000.000,00 (satu milyar rupiah), dengan ketentuan apabila denda tersebut tidak dibayar diganti dengan pidana penjara selama 2 (dua) bulan; 
 Menetapkan masa penangkapan dan penahanan yang telah dijalani oleh Terdakwa dikurangkan seluruhnya dari pidana yang dijatuhkan; 
@@ -1078,6 +1075,9 @@
 Menetapkan barang bukti berupa: 3 (tiga) lembar plastik klip yang didalamnya terdapat narkotika jenis sabu-sabu dengan berat kotor 1,19 gr (satu koma sembilan belas gram) dan berat bersih 0,60 gr (nol koma enam puluh gram); 1 (satu) batang pipet kaca yang didalamnya masih terdapat narkotika jenis sabu-sabu; 1 (satu) buah sendok yang terbuat dari sedotan warna hitam; 1 (satu) lembar plastik klip warna biru; 1 (satu) buah bong terbuat dari kaca; 1 (satu) buah kotak rokok warna putih merah bertuliskan Sampoerna; 1 (satu) buah tas slempang warna hitam; 1 (satu) buah korek api warna merah; Dimusnahkan; 1 (satu) unit sepeda motor R2 merek YAMAHA MIO warna putih dengan nopol DA 6105 QV tanpa surat; 
 Dikembalikan kepada Terdakwa; 1 (satu) unit handphone android merek Samsung warna biru dengan Imei 352384570816670; Dirampas untuk negara; 
 Membebankan kepada Terdakwa membayar biaya perkara sejumlah Rp5.000,00 (lima ribu rupiah);</t>
+  </si>
+  <si>
+    <t>1 (satu) lembar plastik klip yang di dalamnya terdapat narkotika jenis sabu-sabu dengan berat kotor seberat 0,17 gram dan berat bersih seberat 0.04 gram; 10 (sepuluh) lembar plastik Kip; 1 (Satu) buah sendok terbuat dari sedotan plastik warna hitam; dan I (satu) lembar plastik warna hitam; Dimusnahkan</t>
   </si>
 </sst>
 </file>
@@ -1467,8 +1467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAFA8F1-17D9-4523-9FEC-D12F4AEFB99E}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1575,10 +1575,10 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -1586,16 +1586,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -1603,16 +1603,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -1620,16 +1620,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="159.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -1637,16 +1637,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="120" thickBot="1" x14ac:dyDescent="0.35">
@@ -1654,16 +1654,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="186" thickBot="1" x14ac:dyDescent="0.35">
@@ -1671,16 +1671,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="120" thickBot="1" x14ac:dyDescent="0.35">
@@ -1688,16 +1688,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="252" thickBot="1" x14ac:dyDescent="0.35">
@@ -1705,16 +1705,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="212.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1722,16 +1722,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="186" thickBot="1" x14ac:dyDescent="0.35">
@@ -1739,16 +1739,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -1756,16 +1756,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="120" thickBot="1" x14ac:dyDescent="0.35">
@@ -1773,16 +1773,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="159.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -1790,16 +1790,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="159.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -1807,16 +1807,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -1824,16 +1824,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -1841,16 +1841,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="120" thickBot="1" x14ac:dyDescent="0.35">
@@ -1858,16 +1858,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="146.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1875,16 +1875,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -1892,16 +1892,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="146.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1909,16 +1909,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="146.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1926,16 +1926,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -1943,16 +1943,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="186" thickBot="1" x14ac:dyDescent="0.35">
@@ -1960,16 +1960,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -1977,16 +1977,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="159.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -1994,16 +1994,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -2011,16 +2011,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="159.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -2028,16 +2028,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="146.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2045,16 +2045,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -2062,16 +2062,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="172.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -2079,16 +2079,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="146.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2096,16 +2096,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="172.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -2113,16 +2113,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="146.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2130,16 +2130,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="120" thickBot="1" x14ac:dyDescent="0.35">
@@ -2147,16 +2147,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -2164,16 +2164,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -2181,16 +2181,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="120" thickBot="1" x14ac:dyDescent="0.35">
@@ -2198,16 +2198,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -2215,16 +2215,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="172.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -2232,16 +2232,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="199.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2249,16 +2249,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -2266,16 +2266,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -2283,16 +2283,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="146.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2300,16 +2300,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="186" thickBot="1" x14ac:dyDescent="0.35">
@@ -2317,16 +2317,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="186" thickBot="1" x14ac:dyDescent="0.35">
@@ -2334,16 +2334,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>